<commit_message>
Feb 10, 2025, commit #5
</commit_message>
<xml_diff>
--- a/enhancements.xlsx
+++ b/enhancements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/506594a149b35854/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/506594a149b35854/Desktop/Development Projects/ISO 9001 Audit Time Calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_F25DC773A252ABDACC10485E5118603A5ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41D89162-AC26-4FBE-AD1D-DD6F8A0F80A1}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_F25DC773A252ABDACC10485E5118603A5ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74EB93DF-A8FA-45B7-B302-E819030116FE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Enhancement</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>No further enhancements</t>
   </si>
 </sst>
 </file>
@@ -90,18 +93,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -119,6 +119,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,7 +391,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="75.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,93 +406,100 @@
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>